<commit_message>
The thing works now. It is all good.
</commit_message>
<xml_diff>
--- a/Import files/Testing_Assets_import.xlsx
+++ b/Import files/Testing_Assets_import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MzuvukileN\Desktop\Work Folder\Import files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MzuvukileN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="357">
   <si>
     <t>Asset description</t>
   </si>
@@ -1091,10 +1091,7 @@
     <t>Zimbabwe</t>
   </si>
   <si>
-    <t>Vee's Asset</t>
-  </si>
-  <si>
-    <t>Vee</t>
+    <t>Training MiX Import Test</t>
   </si>
 </sst>
 </file>
@@ -1437,12 +1434,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
@@ -1450,7 +1447,7 @@
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" customWidth="1"/>
     <col min="8" max="8" width="8.5703125" customWidth="1"/>
-    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" customWidth="1"/>
     <col min="11" max="11" width="31.5703125" customWidth="1"/>
     <col min="12" max="12" width="32.85546875" customWidth="1"/>
@@ -1482,19 +1479,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
@@ -1534,17 +1531,17 @@
       <c r="A2" t="s">
         <v>356</v>
       </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
       <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>357</v>
+        <v>28</v>
+      </c>
+      <c r="G2">
+        <v>123456789</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>